<commit_message>
change in TO ratio stat column name
</commit_message>
<xml_diff>
--- a/stats/stats_lub_fem_2020.xlsx
+++ b/stats/stats_lub_fem_2020.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>TEAM</t>
   </si>
@@ -94,6 +94,9 @@
     <t>3PT%</t>
   </si>
   <si>
+    <t>PPSA</t>
+  </si>
+  <si>
     <t>eFG%</t>
   </si>
   <si>
@@ -109,10 +112,10 @@
     <t>OREB%</t>
   </si>
   <si>
-    <t>TOV%</t>
-  </si>
-  <si>
-    <t>OppTOV%</t>
+    <t>TOR%</t>
+  </si>
+  <si>
+    <t>OppTOR%</t>
   </si>
   <si>
     <t>FTRate</t>
@@ -512,13 +515,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK12"/>
+  <dimension ref="A1:AL12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,13 +633,16 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:38">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <v>290</v>
@@ -714,42 +720,45 @@
         <v>28.53107344632768</v>
       </c>
       <c r="AB2">
+        <v>2.301533219761499</v>
+      </c>
+      <c r="AC2">
         <v>0.4263202725724021</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>0.3008893280632411</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>0.4442050905979772</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>0.7258261933904528</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>0.289171974522293</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>0.1993786236759058</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>0.2959375840731773</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>0.2614991482112436</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>0.3132411067193676</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:38">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>257</v>
@@ -827,42 +836,45 @@
         <v>21.68284789644013</v>
       </c>
       <c r="AB3">
+        <v>2.286376274328082</v>
+      </c>
+      <c r="AC3">
         <v>0.3943466172381835</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>0.3678728070175439</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>0.4193601856456158</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>0.7015151515151515</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>0.303475935828877</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>0.1953854361162977</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>0.2824356484394234</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>0.2687673772011122</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>0.3421052631578947</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:38">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>212</v>
@@ -940,42 +952,45 @@
         <v>22.51461988304094</v>
       </c>
       <c r="AB4">
+        <v>2.305084745762712</v>
+      </c>
+      <c r="AC4">
         <v>0.3991971454058876</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>0.3585746102449889</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>0.427051246149538</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>0.7281976744186046</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>0.3303684879288437</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>0.1892075985771589</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>0.3134252714129478</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>0.3336306868867083</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>0.3329621380846325</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:38">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>136</v>
@@ -1053,42 +1068,45 @@
         <v>20.75471698113208</v>
       </c>
       <c r="AB5">
+        <v>2.240909090909091</v>
+      </c>
+      <c r="AC5">
         <v>0.3147727272727273</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>0.3584452975047985</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>0.3504718263368413</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>0.6601815823605707</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>0.3290780141843971</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>0.3236947158314949</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>0.230164477086997</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>0.3875</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>0.3243761996161229</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:38">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>95</v>
@@ -1166,42 +1184,45 @@
         <v>13.36898395721925</v>
       </c>
       <c r="AB6">
+        <v>2.215189873417721</v>
+      </c>
+      <c r="AC6">
         <v>0.2019562715765247</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>0.4222508591065292</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>0.2350574247816241</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>0.6095360824742269</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>0.2975420439844761</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>0.3552525226188304</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>0.1936550226958753</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>0.3141542002301496</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>0.2800687285223368</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:38">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>142</v>
@@ -1279,42 +1300,45 @@
         <v>16.6077738515901</v>
       </c>
       <c r="AB7">
+        <v>2.288775510204081</v>
+      </c>
+      <c r="AC7">
         <v>0.2596938775510204</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>0.3519701810436635</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <v>0.2916177673459227</v>
       </c>
-      <c r="AE7">
+      <c r="AF7">
         <v>0.6782729805013927</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>0.2935444579780755</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <v>0.2642664643240273</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <v>0.2706679981079518</v>
       </c>
-      <c r="AI7">
+      <c r="AJ7">
         <v>0.3357142857142857</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <v>0.4142705005324814</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:38">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>150</v>
@@ -1392,42 +1416,45 @@
         <v>19.87179487179487</v>
       </c>
       <c r="AB8">
+        <v>2.354948805460751</v>
+      </c>
+      <c r="AC8">
         <v>0.3515358361774744</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>0.3519091847265222</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>0.3846001740093332</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>0.6980609418282548</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>0.2643504531722055</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>0.2818721422282809</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>0.2382073511896518</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>0.3424345847554039</v>
       </c>
-      <c r="AJ8">
+      <c r="AK8">
         <v>0.3075335397316821</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:38">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9">
         <v>371</v>
@@ -1505,42 +1532,45 @@
         <v>26.12612612612612</v>
       </c>
       <c r="AB9">
+        <v>2.352660841938046</v>
+      </c>
+      <c r="AC9">
         <v>0.4162033359809372</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>0.3180473372781065</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>0.4387020933065179</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>0.7673521850899743</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>0.3645833333333333</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <v>0.1823845476863218</v>
       </c>
-      <c r="AH9">
+      <c r="AI9">
         <v>0.2625533311453889</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <v>0.2764098490865767</v>
       </c>
-      <c r="AJ9">
+      <c r="AK9">
         <v>0.3461538461538461</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:38">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10">
         <v>238</v>
@@ -1618,42 +1648,45 @@
         <v>19.35483870967742</v>
       </c>
       <c r="AB10">
+        <v>2.269799825935596</v>
+      </c>
+      <c r="AC10">
         <v>0.371627502175805</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>0.3345991561181434</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>0.3943726937269373</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>0.711453744493392</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <v>0.3373934226552984</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>0.2497404544930211</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <v>0.2285509292475756</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <v>0.3002610966057441</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>0.2843881856540084</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:38">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>130</v>
@@ -1731,42 +1764,45 @@
         <v>12.57142857142857</v>
       </c>
       <c r="AB11">
+        <v>2.31390134529148</v>
+      </c>
+      <c r="AC11">
         <v>0.252914798206278</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>0.3692028985507246</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>0.2778212552825168</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>0.6059701492537314</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>0.3008474576271186</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>0.3107131297874636</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>0.2003876516788144</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>0.3318385650224215</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>0.336231884057971</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:38">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>269</v>
@@ -1844,33 +1880,36 @@
         <v>28.27225130890053</v>
       </c>
       <c r="AB12">
+        <v>2.343525179856115</v>
+      </c>
+      <c r="AC12">
         <v>0.433453237410072</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>0.3425589836660617</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>0.4669925526372245</v>
       </c>
-      <c r="AE12">
+      <c r="AF12">
         <v>0.7135922330097088</v>
       </c>
-      <c r="AF12">
+      <c r="AG12">
         <v>0.3025099075297226</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>0.2095496499430703</v>
       </c>
-      <c r="AH12">
+      <c r="AI12">
         <v>0.258030987890068</v>
       </c>
-      <c r="AI12">
+      <c r="AJ12">
         <v>0.3947841726618705</v>
       </c>
-      <c r="AJ12">
+      <c r="AK12">
         <v>0.2595281306715064</v>
       </c>
-      <c r="AK12">
+      <c r="AL12">
         <v>16</v>
       </c>
     </row>

</xml_diff>